<commit_message>
10% and 20% misclass data
</commit_message>
<xml_diff>
--- a/Cancer_noisy_SVM.xlsx
+++ b/Cancer_noisy_SVM.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\Documents\GitHub\CancerAceFiltering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD6C81-351C-409A-9C8D-7C28700E2FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD90171E-0055-4A6F-A91F-CD407FC43DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9307C9-804B-42FF-9B1B-186E3C937C4F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DB9307C9-804B-42FF-9B1B-186E3C937C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="10%svm_noisy " sheetId="2" r:id="rId1"/>
     <sheet name="20%_svm_noisy" sheetId="1" r:id="rId2"/>
+    <sheet name="10%_noisy_DT" sheetId="3" r:id="rId3"/>
+    <sheet name="20%_noisy_DT" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'10%_noisy_DT'!$A$1:$L$146</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'10%svm_noisy '!$A$1:$L$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'20%_noisy_DT'!$A$1:$L$146</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'20%_svm_noisy'!$A$1:$L$146</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="13">
   <si>
     <t>PREDICTED</t>
   </si>
@@ -67,17 +71,176 @@
     <t xml:space="preserve">with scaling </t>
   </si>
   <si>
-    <t>param_grid = {'C': [ 1], 'gamma': [0.001, 0.01, 0.1,0.7],'kernel': ['rbf']}</t>
+    <r>
+      <t>classifier =svm.SVC(kernel=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"poly"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, degree=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,  gamma=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"auto"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,C=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,random_state=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
   <si>
-    <t>without scaling</t>
+    <r>
+      <t>max_depth=depth,random_state=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">,min_samples_split = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>max_depth=depth,random_state=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">,min_samples_split = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <t>DT on raw data</t>
+  </si>
+  <si>
+    <t>DT on Curated Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,7 +264,19 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF008000"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFA31515"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF098156"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -309,78 +484,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FAF5AF-2777-4A54-8775-F418F9E41A0F}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,114 +888,114 @@
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="b">
+      <c r="A4" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11">
-        <v>0.96875</v>
-      </c>
-      <c r="D4" s="12">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0.96651799999999999</v>
-      </c>
-      <c r="F4" s="12">
-        <v>3.3481999999999998E-2</v>
+      <c r="C4" s="6">
+        <v>0.984375</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.97842300000000004</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2.1576999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15">
-        <v>2.6911999999999998E-2</v>
-      </c>
-      <c r="D5" s="16">
-        <v>0.97308799999999995</v>
-      </c>
-      <c r="E5" s="15">
-        <v>2.2662999999999999E-2</v>
-      </c>
-      <c r="F5" s="16">
-        <v>0.97733700000000001</v>
+      <c r="C5" s="9">
+        <v>7.3653999999999997E-2</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.926346</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5.3823999999999997E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.94617600000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20">
-        <v>0.97308799999999995</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20">
-        <v>0.97733700000000001</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="15">
+        <v>0.926346</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="15">
+        <v>0.94617600000000002</v>
+      </c>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="20">
-        <v>3.125E-2</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="24">
-        <v>3.3481999999999998E-2</v>
-      </c>
-      <c r="F8" s="25"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17">
+        <v>2.1576999999999999E-2</v>
+      </c>
+      <c r="F8" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
@@ -828,7 +1003,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -856,7 +1031,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,122 +1045,426 @@
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="b">
+      <c r="A4" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11">
-        <v>0.97321400000000002</v>
-      </c>
-      <c r="D4" s="12">
-        <v>2.6786000000000001E-2</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0.96503000000000005</v>
-      </c>
-      <c r="F4" s="12">
-        <v>3.4970000000000001E-2</v>
+      <c r="C4" s="6">
+        <v>0.98288699999999996</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1.7113E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.97544600000000004</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2.4553999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15">
-        <v>3.9660000000000001E-2</v>
-      </c>
-      <c r="D5" s="16">
-        <v>0.96033999999999997</v>
-      </c>
-      <c r="E5" s="15">
-        <v>1.6997000000000002E-2</v>
-      </c>
-      <c r="F5" s="16">
-        <v>0.98300299999999996</v>
+      <c r="C5" s="9">
+        <v>7.9320000000000002E-2</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.92068000000000005</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5.9490000000000001E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.94050999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20">
-        <v>0.96033999999999997</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20">
-        <v>0.98300299999999996</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="15">
+        <v>0.92068000000000005</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="15">
+        <v>0.94050999999999996</v>
+      </c>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="20">
-        <v>2.6786000000000001E-2</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="20">
-        <v>3.4970000000000001E-2</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15">
+        <v>1.7113E-2</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17">
+        <v>2.4553999999999999E-2</v>
+      </c>
+      <c r="F8" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="26" t="s">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="12" t="s">
         <v>8</v>
       </c>
     </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68046DD1-FE5A-4360-A411-B074F13E641E}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.97</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.97</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="24"/>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.13</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.87</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="17">
+        <v>0.87</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9587ABB3-4ECD-4C37-A1ED-1A9D5496E770}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.97</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.97</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="24"/>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.86</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="15">
+        <v>0.86</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="15">
+        <v>0.88</v>
+      </c>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="F8" s="18"/>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+      <c r="C14" s="12" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>